<commit_message>
add feature: draw connecting line between two room node
</commit_message>
<xml_diff>
--- a/documents/20183791_Nguyễn-Hoàng-Long_PGNV-DATN_27.10.2023.xlsx
+++ b/documents/20183791_Nguyễn-Hoàng-Long_PGNV-DATN_27.10.2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longk\OneDrive\Desktop\study\20231\datn\escape-from-dungeon\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1996D96-5B0C-4209-AC49-A0EBB45184AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E092939B-7114-40E8-8753-7DDD350BC110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="822" xr2:uid="{A4C764ED-A697-7E4F-AB21-1130AE3D2115}"/>
   </bookViews>
@@ -3367,7 +3367,7 @@
   </sheetPr>
   <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="144" workbookViewId="0">
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A35" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="144" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:K28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add feature: add entrance node in first create room node and selected other graph in RoomNodeGraphs asset
</commit_message>
<xml_diff>
--- a/documents/20183791_Nguyễn-Hoàng-Long_PGNV-DATN_27.10.2023.xlsx
+++ b/documents/20183791_Nguyễn-Hoàng-Long_PGNV-DATN_27.10.2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longk\OneDrive\Desktop\study\20231\datn\escape-from-dungeon\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E092939B-7114-40E8-8753-7DDD350BC110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8065ABEA-24E3-4D2D-8FF2-85213EB19DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="822" xr2:uid="{A4C764ED-A697-7E4F-AB21-1130AE3D2115}"/>
   </bookViews>
@@ -3367,8 +3367,8 @@
   </sheetPr>
   <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A35" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="144" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:K28"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="144" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="14.25"/>
@@ -4044,13 +4044,13 @@
         <v>38</v>
       </c>
       <c r="I50" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K50" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -4111,13 +4111,13 @@
         <v>38</v>
       </c>
       <c r="I55" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K55" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -4174,7 +4174,7 @@
         <v>38</v>
       </c>
       <c r="I60" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J60" s="5" t="s">
         <v>39</v>

</xml_diff>